<commit_message>
add rank to report
</commit_message>
<xml_diff>
--- a/foy2023-tw.xlsx
+++ b/foy2023-tw.xlsx
@@ -8,43 +8,46 @@
   </bookViews>
   <sheets>
     <sheet name="順位" sheetId="1" r:id="rId1"/>
-    <sheet name="0331418A" sheetId="2" r:id="rId5"/>
-    <sheet name="03311187" sheetId="3" r:id="rId6"/>
-    <sheet name="2931113C" sheetId="4" r:id="rId7"/>
-    <sheet name="25311177" sheetId="5" r:id="rId8"/>
-    <sheet name="29313233" sheetId="6" r:id="rId9"/>
-    <sheet name="9N311091" sheetId="7" r:id="rId10"/>
-    <sheet name="01312237" sheetId="8" r:id="rId11"/>
-    <sheet name="03312175" sheetId="9" r:id="rId12"/>
-    <sheet name="03312184" sheetId="10" r:id="rId13"/>
-    <sheet name="03319172" sheetId="11" r:id="rId14"/>
-    <sheet name="04311181" sheetId="12" r:id="rId15"/>
-    <sheet name="4731B15C" sheetId="13" r:id="rId16"/>
-    <sheet name="9Q311103" sheetId="14" r:id="rId17"/>
-    <sheet name="03311112" sheetId="15" r:id="rId18"/>
-    <sheet name="03316183" sheetId="16" r:id="rId19"/>
-    <sheet name="04317188" sheetId="17" r:id="rId20"/>
-    <sheet name="1494" sheetId="18" r:id="rId21"/>
-    <sheet name="29313158" sheetId="19" r:id="rId22"/>
-    <sheet name="4231111C" sheetId="20" r:id="rId23"/>
-    <sheet name="80311083" sheetId="21" r:id="rId24"/>
-    <sheet name="89311239" sheetId="22" r:id="rId25"/>
-    <sheet name="91311179" sheetId="23" r:id="rId26"/>
-    <sheet name="96311073" sheetId="24" r:id="rId27"/>
-    <sheet name="9C31108A" sheetId="25" r:id="rId28"/>
-    <sheet name="9I311179" sheetId="26" r:id="rId29"/>
-    <sheet name="9I311187" sheetId="27" r:id="rId30"/>
-    <sheet name="9I312187" sheetId="28" r:id="rId31"/>
-    <sheet name="AY311227" sheetId="29" r:id="rId32"/>
-    <sheet name="Tracers" sheetId="30" r:id="rId33"/>
-    <sheet name="VYM" sheetId="31" r:id="rId34"/>
+    <sheet name="1_0331418A" sheetId="2" r:id="rId5"/>
+    <sheet name="2_03311187" sheetId="3" r:id="rId6"/>
+    <sheet name="3_2931113C" sheetId="4" r:id="rId7"/>
+    <sheet name="4_25311177" sheetId="5" r:id="rId8"/>
+    <sheet name="5_29313233" sheetId="6" r:id="rId9"/>
+    <sheet name="5_9N311091" sheetId="7" r:id="rId10"/>
+    <sheet name="7_01312237" sheetId="8" r:id="rId11"/>
+    <sheet name="7_03312175" sheetId="9" r:id="rId12"/>
+    <sheet name="7_03312184" sheetId="10" r:id="rId13"/>
+    <sheet name="7_03319172" sheetId="11" r:id="rId14"/>
+    <sheet name="7_04311181" sheetId="12" r:id="rId15"/>
+    <sheet name="7_4731B15C" sheetId="13" r:id="rId16"/>
+    <sheet name="7_9Q311103" sheetId="14" r:id="rId17"/>
+    <sheet name="14_03311112" sheetId="15" r:id="rId18"/>
+    <sheet name="14_03316183" sheetId="16" r:id="rId19"/>
+    <sheet name="14_04317188" sheetId="17" r:id="rId20"/>
+    <sheet name="14_1494" sheetId="18" r:id="rId21"/>
+    <sheet name="14_29313158" sheetId="19" r:id="rId22"/>
+    <sheet name="14_4231111C" sheetId="20" r:id="rId23"/>
+    <sheet name="14_80311083" sheetId="21" r:id="rId24"/>
+    <sheet name="14_89311239" sheetId="22" r:id="rId25"/>
+    <sheet name="14_91311179" sheetId="23" r:id="rId26"/>
+    <sheet name="14_96311073" sheetId="24" r:id="rId27"/>
+    <sheet name="14_9C31108A" sheetId="25" r:id="rId28"/>
+    <sheet name="14_9I311179" sheetId="26" r:id="rId29"/>
+    <sheet name="14_9I311187" sheetId="27" r:id="rId30"/>
+    <sheet name="14_9I312187" sheetId="28" r:id="rId31"/>
+    <sheet name="14_AY311227" sheetId="29" r:id="rId32"/>
+    <sheet name="14_Tracers" sheetId="30" r:id="rId33"/>
+    <sheet name="14_VYM" sheetId="31" r:id="rId34"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
+  <si>
+    <t>順位</t>
+  </si>
   <si>
     <t>票数</t>
   </si>
@@ -52,6 +55,9 @@
     <t>ファンド名</t>
   </si>
   <si>
+    <t>コメント</t>
+  </si>
+  <si>
     <t>0331418A eMAXIS Slim 全世界株式(オール・カントリー) 三菱UFJアセットマネジメント</t>
   </si>
   <si>
@@ -64,94 +70,91 @@
     <t>25311177 農林中金&lt;パートナーズ&gt;長期厳選投資 おおぶね 農林中金全共連アセットマネジメント</t>
   </si>
   <si>
+    <t>29313233 &lt;購入・換金手数料なし&gt;ニッセイNASDAQ100インデックスファンド ニッセイアセットマネジメント</t>
+  </si>
+  <si>
     <t>9N311091 コモンズ30ファンド コモンズ投信</t>
   </si>
   <si>
-    <t>29313233 &lt;購入・換金手数料なし&gt;ニッセイNASDAQ100インデックスファンド ニッセイアセットマネジメント</t>
+    <t>01312237 はじめてのNISA・全世界株式インデックス(オール・カントリー) 野村アセットマネジメント</t>
+  </si>
+  <si>
+    <t>03312175 eMAXIS Slim バランス(8資産均等型) 三菱UFJアセットマネジメント</t>
+  </si>
+  <si>
+    <t>03312184 eMAXIS Slim 全世界株式(3地域均等型) 三菱UFJアセットマネジメント</t>
+  </si>
+  <si>
+    <t>03319172 eMAXIS Slim 先進国株式インデックス 三菱UFJアセットマネジメント</t>
+  </si>
+  <si>
+    <t>04311181 iFreeNEXT FANG+インデックス 大和アセットマネジメント</t>
+  </si>
+  <si>
+    <t>4731B15C たわらノーロード 先進国株式 アセットマネジメントOne</t>
   </si>
   <si>
     <t>9Q311103 結い 2101 鎌倉投信</t>
   </si>
   <si>
-    <t>4731B15C たわらノーロード 先進国株式 アセットマネジメントOne</t>
-  </si>
-  <si>
-    <t>04311181 iFreeNEXT FANG+インデックス 大和アセットマネジメント</t>
-  </si>
-  <si>
-    <t>03319172 eMAXIS Slim 先進国株式インデックス 三菱UFJアセットマネジメント</t>
-  </si>
-  <si>
-    <t>03312184 eMAXIS Slim 全世界株式(3地域均等型) 三菱UFJアセットマネジメント</t>
-  </si>
-  <si>
-    <t>03312175 eMAXIS Slim バランス(8資産均等型) 三菱UFJアセットマネジメント</t>
-  </si>
-  <si>
-    <t>01312237 はじめてのNISA・全世界株式インデックス(オール・カントリー) 野村アセットマネジメント</t>
+    <t>03311112 三菱UFJ 純金ファンド 三菱UFJアセットマネジメント</t>
+  </si>
+  <si>
+    <t>03316183 eMAXIS Slim 全世界株式(除く日本) 三菱UFJアセットマネジメント</t>
+  </si>
+  <si>
+    <t>04317188 iFreeNEXT NASDAQ100インデックス 大和アセットマネジメント</t>
+  </si>
+  <si>
+    <t>1494 One ETF 高配当日本株 アセットマネジメントOne</t>
+  </si>
+  <si>
+    <t>29313158 &lt;購入・換金手数料なし&gt;ニッセイ・インデックスバランスファンド(4資産均等型) ニッセイアセットマネジメント</t>
+  </si>
+  <si>
+    <t>4231111C ピクテ・ゴールド(為替ヘッジあり) ピクテ･ジャパン</t>
+  </si>
+  <si>
+    <t>80311083 スパークス・新・国際優良日本株ファンド スパークス･アセット･マネジメント</t>
+  </si>
+  <si>
+    <t>89311239 SBI・iシェアーズ・インド株式インデックス・ファンド SBIアセットマネジメント</t>
+  </si>
+  <si>
+    <t>91311179 TORANOTECアクティブジャパン TORANOTEC投信投資顧問</t>
+  </si>
+  <si>
+    <t>96311073 セゾン・グローバルバランスファンド セゾン投信</t>
+  </si>
+  <si>
+    <t>9C31108A ひふみ投信 レオス･キャピタルワークス</t>
+  </si>
+  <si>
+    <t>9I311179 楽天・全世界株式インデックス・ファンド 楽天投信投資顧問</t>
+  </si>
+  <si>
+    <t>9I311187 楽天・インデックス・バランス・ファンド(株式重視型) 楽天投信投資顧問</t>
+  </si>
+  <si>
+    <t>9I312187 楽天・インデックス・バランス・ファンド(均等型) 楽天投信投資顧問</t>
+  </si>
+  <si>
+    <t>AY311227 auAMレバレッジ NASDAQ100 auアセットマネジメント</t>
+  </si>
+  <si>
+    <t>Tracers S&amp;P500配当貴族インデックス(米国株式) 日興アセットマネジメント</t>
   </si>
   <si>
     <t>VYM バンガード・ 米国高配当株式ETF バンガード グループ</t>
   </si>
   <si>
-    <t>Tracers S&amp;P500配当貴族インデックス(米国株式) 日興アセットマネジメント</t>
-  </si>
-  <si>
-    <t>AY311227 auAMレバレッジ NASDAQ100 auアセットマネジメント</t>
-  </si>
-  <si>
-    <t>9I312187 楽天・インデックス・バランス・ファンド(均等型) 楽天投信投資顧問</t>
-  </si>
-  <si>
-    <t>9I311187 楽天・インデックス・バランス・ファンド(株式重視型) 楽天投信投資顧問</t>
-  </si>
-  <si>
-    <t>9I311179 楽天・全世界株式インデックス・ファンド 楽天投信投資顧問</t>
-  </si>
-  <si>
-    <t>9C31108A ひふみ投信 レオス･キャピタルワークス</t>
-  </si>
-  <si>
-    <t>96311073 セゾン・グローバルバランスファンド セゾン投信</t>
-  </si>
-  <si>
-    <t>91311179 TORANOTECアクティブジャパン TORANOTEC投信投資顧問</t>
-  </si>
-  <si>
-    <t>89311239 SBI・iシェアーズ・インド株式インデックス・ファンド SBIアセットマネジメント</t>
-  </si>
-  <si>
-    <t>80311083 スパークス・新・国際優良日本株ファンド スパークス･アセット･マネジメント</t>
-  </si>
-  <si>
-    <t>4231111C ピクテ・ゴールド(為替ヘッジあり) ピクテ･ジャパン</t>
-  </si>
-  <si>
-    <t>29313158 &lt;購入・換金手数料なし&gt;ニッセイ・インデックスバランスファンド(4資産均等型) ニッセイアセットマネジメント</t>
-  </si>
-  <si>
-    <t>1494 One ETF 高配当日本株 アセットマネジメントOne</t>
-  </si>
-  <si>
-    <t>04317188 iFreeNEXT NASDAQ100インデックス 大和アセットマネジメント</t>
-  </si>
-  <si>
-    <t>03316183 eMAXIS Slim 全世界株式(除く日本) 三菱UFJアセットマネジメント</t>
-  </si>
-  <si>
-    <t>03311112 三菱UFJ 純金ファンド 三菱UFJアセットマネジメント</t>
-  </si>
-  <si>
-    <t>票</t>
+    <t>1</t>
   </si>
   <si>
     <t>名前</t>
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>コメント</t>
   </si>
   <si>
     <t>時刻</t>
@@ -498,6 +501,9 @@
     <t>2023-11-30 23:59:01</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>バルーン</t>
   </si>
   <si>
@@ -574,6 +580,9 @@
   </si>
   <si>
     <t>2023-11-30 21:34:39</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>ももんが</t>
@@ -641,6 +650,9 @@
     <t>2023-11-30 12:12:50</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>大空みさき@のんびりコツコツ投資生活</t>
   </si>
   <si>
@@ -687,6 +699,9 @@
   </si>
   <si>
     <t>2023-11-30 22:19:50</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t>50代からの投資</t>
@@ -768,6 +783,9 @@
     <t>2023-11-26 22:13:22</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>kawffie</t>
   </si>
   <si>
@@ -936,6 +954,9 @@
   </si>
   <si>
     <t>2023-11-29 20:36:39</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
   <si>
     <t>銀行で投信</t>
@@ -1478,7 +1499,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col customWidth="true" max="2" min="2" width="91.4"/>
+    <col customWidth="true" max="3" min="3" width="91.4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1488,245 +1509,341 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>1</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>1</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1">
-        <v>1</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1">
-        <v>1</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>29</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1">
-        <v>1</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>1</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1740,63 +1857,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>2</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>230</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="45" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>241</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="true">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="45" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>243</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -1810,63 +1934,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>247</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>248</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="true">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>252</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1880,63 +2011,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>256</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>257</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1950,63 +2088,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>264</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" ht="45" customHeight="true">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" ht="45" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2020,63 +2165,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>270</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>271</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="true">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>275</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2090,49 +2242,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>278</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>279</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>280</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -2146,49 +2305,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>283</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>284</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2202,49 +2368,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>287</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>288</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2258,49 +2431,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>291</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>292</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2314,49 +2494,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>295</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>296</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2370,413 +2557,420 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>27</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" ht="30" customHeight="true">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="true">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="8" ht="30" customHeight="true">
+      <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" ht="45" customHeight="true">
-      <c r="A8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="1" t="s">
+    </row>
+    <row r="9" ht="45" customHeight="true">
+      <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" ht="30" customHeight="true">
-      <c r="A9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="10" ht="30" customHeight="true">
+      <c r="A10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" ht="45" customHeight="true">
-      <c r="A10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11" ht="45" customHeight="true">
+      <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" ht="30" customHeight="true">
-      <c r="A11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="true">
       <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="true">
       <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" ht="30" customHeight="true">
+      <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" ht="30" customHeight="true">
-      <c r="A15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" ht="30" customHeight="true">
+      <c r="A16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="18" ht="30" customHeight="true">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="true">
       <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="true">
       <c r="A20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" ht="30" customHeight="true">
+      <c r="A21" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="21" ht="60" customHeight="true">
-      <c r="A21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="60" customHeight="true">
+      <c r="A22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="22" ht="30" customHeight="true">
-      <c r="A22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="true">
       <c r="A23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="true">
       <c r="A24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="true">
       <c r="A25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="true">
       <c r="A26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="27" ht="30" customHeight="true">
+      <c r="A27" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="1" t="s">
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" ht="30" customHeight="true">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="true">
       <c r="A29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="1" t="s">
+    </row>
+    <row r="30" ht="30" customHeight="true">
+      <c r="A30" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>141</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2790,49 +2984,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>299</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>300</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2846,49 +3047,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>302</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>303</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>304</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2902,49 +3110,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>306</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>307</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>308</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -2958,49 +3173,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>311</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>312</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3014,49 +3236,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>315</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>316</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3070,49 +3299,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>317</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>318</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3126,49 +3362,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>321</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>322</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -3182,49 +3425,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>325</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>326</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -3238,49 +3488,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>328</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>329</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>330</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -3294,49 +3551,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>332</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>334</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -3350,119 +3614,126 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>145</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="true">
       <c r="A5" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="true">
       <c r="A6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="true">
       <c r="A7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="true">
       <c r="A8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C8" s="1" t="s">
+    </row>
+    <row r="9" ht="30" customHeight="true">
+      <c r="A9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3476,49 +3747,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>337</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>338</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3532,49 +3810,56 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>341</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>342</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="30" customHeight="true">
+      <c r="A4" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3588,105 +3873,112 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="true">
       <c r="A5" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="true">
       <c r="A6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="true">
       <c r="A7" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="8" ht="30" customHeight="true">
+      <c r="A8" s="1" t="s">
         <v>185</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -3700,49 +3992,42 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>188</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
@@ -3759,7 +4044,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" ht="30" customHeight="true">
       <c r="A5" s="1" t="s">
         <v>194</v>
       </c>
@@ -3767,24 +4052,38 @@
         <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>196</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" ht="30" customHeight="true">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>199</v>
+        <v>48</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="7" ht="30" customHeight="true">
+      <c r="A7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3798,77 +4097,84 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>203</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>204</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="true">
       <c r="A5" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="true">
+      <c r="A6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -3882,77 +4188,84 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="45" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>215</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="true">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" ht="45" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="true">
       <c r="A5" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" ht="30" customHeight="true">
+      <c r="A6" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3966,63 +4279,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>227</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>228</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4036,63 +4356,70 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col customWidth="true" max="1" min="1" width="27.42"/>
-    <col customWidth="true" max="2" min="2" width="22.85"/>
-    <col customWidth="true" max="3" min="3" width="109.68"/>
-    <col customWidth="true" max="4" min="4" width="22.85"/>
+    <col customWidth="true" max="2" min="1" width="22.85"/>
+    <col customWidth="true" max="3" min="3" width="114.25"/>
+    <col customWidth="true" max="4" min="4" width="27.42"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" ht="30" customHeight="true">
-      <c r="A3" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>235</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>236</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="true">
       <c r="A4" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" ht="30" customHeight="true">
+      <c r="A5" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>